<commit_message>
TS 1.1 Kampam 15/07/2020
</commit_message>
<xml_diff>
--- a/padam_excel/TS 1.1 Padam Input Template.xlsx
+++ b/padam_excel/TS 1.1 Padam Input Template.xlsx
@@ -4020,9 +4020,9 @@
   <dimension ref="A1:AD1581"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A390" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="R398" sqref="R398"/>
+      <selection pane="bottomLeft" activeCell="M269" sqref="M269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>